<commit_message>
Correcting and added first actual test for checkbox
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/alx.xlsx
+++ b/src/test/resources/xls/alx.xlsx
@@ -8,14 +8,15 @@
     <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
     <sheet name="GSMArena" sheetId="2" r:id="rId5"/>
     <sheet name="Amazon" sheetId="3" r:id="rId6"/>
-    <sheet name="Calculator" sheetId="4" r:id="rId7"/>
-    <sheet name="Data" sheetId="5" r:id="rId8"/>
+    <sheet name="Amz-CB" sheetId="4" r:id="rId7"/>
+    <sheet name="Calculator" sheetId="5" r:id="rId8"/>
+    <sheet name="Data" sheetId="6" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -29,10 +30,80 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>GSMArena</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>GSMArena</t>
+    </r>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Amazon</t>
+    </r>
+  </si>
+  <si>
+    <t>Amz-CB</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Amz-CB</t>
+    </r>
+  </si>
+  <si>
+    <t>Calculator</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Calculator</t>
+    </r>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Data</t>
+    </r>
   </si>
   <si>
     <t>Execute</t>
@@ -116,9 +187,6 @@
     <t>12000mAh</t>
   </si>
   <si>
-    <t>Amazon</t>
-  </si>
-  <si>
     <t>TestID</t>
   </si>
   <si>
@@ -146,7 +214,49 @@
     <t>%^&amp;**()_{}</t>
   </si>
   <si>
-    <t>Calculator</t>
+    <t>checkbox</t>
+  </si>
+  <si>
+    <t>CB01</t>
+  </si>
+  <si>
+    <t>Seagate</t>
+  </si>
+  <si>
+    <t>CB02</t>
+  </si>
+  <si>
+    <t>Gotega</t>
+  </si>
+  <si>
+    <t>CB03</t>
+  </si>
+  <si>
+    <t>Rioddas</t>
+  </si>
+  <si>
+    <t>CB04</t>
+  </si>
+  <si>
+    <t>Western Digital</t>
+  </si>
+  <si>
+    <t>CB05</t>
+  </si>
+  <si>
+    <t>Samsung Electronics</t>
+  </si>
+  <si>
+    <t>CB06</t>
+  </si>
+  <si>
+    <t>Kingston</t>
+  </si>
+  <si>
+    <t>CB07</t>
+  </si>
+  <si>
+    <t>SanDisk</t>
   </si>
   <si>
     <t>a</t>
@@ -183,9 +293,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>Data</t>
   </si>
   <si>
     <t>TestTitle</t>
@@ -322,11 +429,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="14"/>
+      <color indexed="16"/>
       <name val="Menlo Regular"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,19 +460,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="18"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="19"/>
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -375,133 +482,25 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="21"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="24">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="17"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="17"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="17"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="17"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="17"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -532,9 +531,7 @@
       <top style="thin">
         <color indexed="13"/>
       </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -548,10 +545,227 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="13"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="19"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="19"/>
+      </right>
+      <top style="thin">
+        <color indexed="19"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="19"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="19"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="19"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="19"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="19"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
       <bottom style="thin">
         <color indexed="13"/>
       </bottom>
@@ -576,7 +790,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -598,100 +812,172 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -716,6 +1002,8 @@
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff222222"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
@@ -873,9 +1161,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -955,7 +1243,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -983,10 +1271,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1242,9 +1530,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1532,7 +1820,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1560,10 +1848,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1814,107 +2102,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="0.05" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="10"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>6</v>
+      </c>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="10"/>
       <c r="B13" t="s" s="3">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="10"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>8</v>
+      </c>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" ht="13" customHeight="1">
+      <c r="A15" s="10"/>
       <c r="B15" t="s" s="3">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-    </row>
-    <row r="16">
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" ht="13" customHeight="1">
+      <c r="A16" s="20"/>
       <c r="B16" s="4"/>
       <c r="C16" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>56</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" ht="13" customHeight="1">
+      <c r="A17" s="7"/>
+      <c r="B17" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" ht="13" customHeight="1">
+      <c r="A18" s="10"/>
+      <c r="B18" s="4"/>
+      <c r="C18" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" ht="13" customHeight="1">
+      <c r="A19" s="10"/>
+      <c r="B19" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" ht="13" customHeight="1">
+      <c r="A20" s="20"/>
+      <c r="B20" s="4"/>
+      <c r="C20" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="E20" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'GSMArena'!R1C1" tooltip="" display="GSMArena"/>
-    <hyperlink ref="D12" location="'Amazon'!R1C1" tooltip="" display="Amazon"/>
-    <hyperlink ref="D14" location="'Calculator'!R1C1" tooltip="" display="Calculator"/>
-    <hyperlink ref="D16" location="'Data'!R1C1" tooltip="" display="Data"/>
+    <hyperlink ref="D12" location="'GSMArena'!R1C1" tooltip="" display="GSMArena"/>
+    <hyperlink ref="D14" location="'Amazon'!R1C1" tooltip="" display="Amazon"/>
+    <hyperlink ref="D16" location="'Amz-CB'!R1C1" tooltip="" display="Amz-CB"/>
+    <hyperlink ref="D18" location="'Calculator'!R1C1" tooltip="" display="Calculator"/>
+    <hyperlink ref="D20" location="'Data'!R1C1" tooltip="" display="Data"/>
+    <hyperlink ref="D12" location="'GSMArena'!R1C1" tooltip="" display="GSMArena"/>
+    <hyperlink ref="D14" location="'Amazon'!R1C1" tooltip="" display="Amazon"/>
+    <hyperlink ref="D16" location="'Amz-CB'!R1C1" tooltip="" display="Amz-CB"/>
+    <hyperlink ref="D18" location="'Calculator'!R1C1" tooltip="" display="Calculator"/>
+    <hyperlink ref="D20" location="'Data'!R1C1" tooltip="" display="Data"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1926,190 +2340,190 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.3516" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="6" customWidth="1"/>
-    <col min="6" max="6" width="10.1719" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.8516" style="6" customWidth="1"/>
-    <col min="8" max="9" width="8.85156" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="25" customWidth="1"/>
+    <col min="2" max="2" width="15.3516" style="25" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="25" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="25" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="25" customWidth="1"/>
+    <col min="6" max="6" width="10.1719" style="25" customWidth="1"/>
+    <col min="7" max="7" width="11.8516" style="25" customWidth="1"/>
+    <col min="8" max="9" width="8.85156" style="25" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="I1" s="8"/>
+      <c r="A1" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s" s="26">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s" s="26">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s" s="26">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s" s="26">
+        <v>23</v>
+      </c>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" ht="16" customHeight="1">
-      <c r="A2" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s" s="9">
-        <v>21</v>
-      </c>
-      <c r="I2" s="11"/>
+      <c r="A2" t="s" s="28">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s" s="28">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s" s="28">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s" s="29">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s" s="28">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s" s="28">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s" s="28">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s" s="28">
+        <v>31</v>
+      </c>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s" s="9">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s" s="9">
+      <c r="A3" t="s" s="28">
         <v>24</v>
       </c>
-      <c r="F3" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s" s="9">
+      <c r="B3" t="s" s="28">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s" s="28">
         <v>26</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="D3" t="s" s="28">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s" s="28">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s" s="28">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s" s="28">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s" s="28">
+        <v>36</v>
+      </c>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s" s="9">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="I4" s="11"/>
+      <c r="A4" t="s" s="28">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s" s="28">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s" s="28">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s" s="28">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s" s="28">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s" s="28">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s" s="28">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s" s="28">
+        <v>42</v>
+      </c>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2125,101 +2539,115 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="4" width="16.3516" style="12" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="12" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
-      <c r="A1" t="s" s="13">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="13">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s" s="13">
-        <v>35</v>
-      </c>
-      <c r="D1" s="14"/>
+      <c r="A1" t="s" s="32">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="32">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s" s="32">
+        <v>44</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" ht="13.1" customHeight="1">
-      <c r="A2" t="s" s="15">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s" s="16">
-        <v>36</v>
-      </c>
-      <c r="C2" s="17">
+      <c r="A2" t="s" s="35">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s" s="36">
+        <v>45</v>
+      </c>
+      <c r="C2" s="37">
         <v>1234567</v>
       </c>
-      <c r="D2" s="18"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" ht="12.9" customHeight="1">
-      <c r="A3" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s" s="20">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s" s="21">
-        <v>38</v>
-      </c>
-      <c r="D3" s="22"/>
+      <c r="A3" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s" s="41">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s" s="42">
+        <v>47</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" ht="12.9" customHeight="1">
-      <c r="A4" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s" s="20">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s" s="21">
-        <v>40</v>
-      </c>
-      <c r="D4" s="22"/>
+      <c r="A4" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s" s="41">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s" s="42">
+        <v>49</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" ht="12.9" customHeight="1">
-      <c r="A5" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="20">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s" s="21">
-        <v>42</v>
-      </c>
-      <c r="D5" s="22"/>
+      <c r="A5" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s" s="41">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s" s="42">
+        <v>51</v>
+      </c>
+      <c r="D5" s="43"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" ht="12.9" customHeight="1">
-      <c r="A6" s="23"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" ht="12.9" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" ht="12.9" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" ht="12.9" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="39"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -2232,129 +2660,241 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="3" width="16.3516" style="48" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="48" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.1" customHeight="1">
+      <c r="A1" t="s" s="32">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="32">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s" s="32">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" ht="13.1" customHeight="1">
+      <c r="A2" t="s" s="35">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s" s="36">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s" s="49">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" ht="12.9" customHeight="1">
+      <c r="A3" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s" s="41">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s" s="42">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" ht="12.9" customHeight="1">
+      <c r="A4" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s" s="41">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s" s="42">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" ht="12.9" customHeight="1">
+      <c r="A5" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s" s="41">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s" s="42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" ht="12.9" customHeight="1">
+      <c r="A6" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s" s="41">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s" s="42">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" ht="12.9" customHeight="1">
+      <c r="A7" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="41">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s" s="42">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" ht="12.9" customHeight="1">
+      <c r="A8" t="s" s="40">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s" s="41">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s" s="42">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="25" customWidth="1"/>
-    <col min="2" max="2" width="11.3516" style="25" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="25" customWidth="1"/>
-    <col min="4" max="4" width="12.8516" style="25" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="25" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="50" customWidth="1"/>
+    <col min="2" max="2" width="11.3516" style="50" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="50" customWidth="1"/>
+    <col min="4" max="4" width="12.8516" style="50" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="50" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E1" t="s" s="7">
-        <v>46</v>
+      <c r="A1" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="26">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s" s="26">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s" s="26">
+        <v>69</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s" s="9">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>49</v>
-      </c>
-      <c r="E2" s="26">
+      <c r="A2" t="s" s="28">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s" s="28">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s" s="28">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s" s="28">
+        <v>72</v>
+      </c>
+      <c r="E2" s="51">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s" s="9">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s" s="9">
-        <v>52</v>
-      </c>
-      <c r="E3" s="26">
+      <c r="A3" t="s" s="28">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s" s="28">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s" s="28">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s" s="28">
+        <v>75</v>
+      </c>
+      <c r="E3" s="51">
         <v>23</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>55</v>
-      </c>
-      <c r="E4" s="26">
+      <c r="A4" t="s" s="28">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s" s="28">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s" s="28">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s" s="28">
+        <v>78</v>
+      </c>
+      <c r="E4" s="51">
         <v>100</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2365,7 +2905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -2373,261 +2913,261 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.17188" style="27" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="27" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="27" customWidth="1"/>
-    <col min="4" max="4" width="20.3516" style="27" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="27" customWidth="1"/>
+    <col min="1" max="1" width="7.17188" style="52" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="52" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="52" customWidth="1"/>
+    <col min="4" max="4" width="20.3516" style="52" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="52" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="28">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="29">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="29">
-        <v>57</v>
-      </c>
-      <c r="D1" t="s" s="29">
-        <v>58</v>
-      </c>
-      <c r="E1" s="30"/>
+      <c r="A1" t="s" s="53">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="54">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="54">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s" s="54">
+        <v>80</v>
+      </c>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s" s="32">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s" s="33">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s" s="33">
-        <v>61</v>
-      </c>
-      <c r="E2" s="8"/>
+      <c r="A2" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s" s="57">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s" s="58">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s" s="58">
+        <v>83</v>
+      </c>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s" s="34">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s" s="35">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s" s="35">
-        <v>64</v>
-      </c>
-      <c r="E3" s="8"/>
+      <c r="A3" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s" s="59">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s" s="60">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s" s="60">
+        <v>86</v>
+      </c>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s" s="34">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s" s="35">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s" s="35">
-        <v>67</v>
-      </c>
-      <c r="E4" s="8"/>
+      <c r="A4" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s" s="59">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s" s="60">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s" s="60">
+        <v>89</v>
+      </c>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="34">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s" s="35">
-        <v>69</v>
-      </c>
-      <c r="D5" t="s" s="35">
-        <v>70</v>
-      </c>
-      <c r="E5" s="8"/>
+      <c r="A5" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s" s="59">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s" s="60">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s" s="60">
+        <v>92</v>
+      </c>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s" s="34">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s" s="35">
-        <v>72</v>
-      </c>
-      <c r="D6" t="s" s="35">
-        <v>73</v>
-      </c>
-      <c r="E6" s="8"/>
+      <c r="A6" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s" s="59">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s" s="60">
+        <v>94</v>
+      </c>
+      <c r="D6" t="s" s="60">
+        <v>95</v>
+      </c>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s" s="34">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s" s="35">
-        <v>75</v>
-      </c>
-      <c r="D7" t="s" s="35">
-        <v>76</v>
-      </c>
-      <c r="E7" s="8"/>
+      <c r="A7" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="59">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s" s="60">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s" s="60">
+        <v>98</v>
+      </c>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s" s="34">
-        <v>77</v>
-      </c>
-      <c r="C8" t="s" s="35">
-        <v>78</v>
-      </c>
-      <c r="D8" t="s" s="35">
-        <v>79</v>
-      </c>
-      <c r="E8" s="8"/>
+      <c r="A8" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s" s="59">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s" s="60">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s" s="60">
+        <v>101</v>
+      </c>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s" s="34">
-        <v>80</v>
-      </c>
-      <c r="C9" t="s" s="35">
-        <v>81</v>
-      </c>
-      <c r="D9" t="s" s="35">
-        <v>82</v>
-      </c>
-      <c r="E9" s="8"/>
+      <c r="A9" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s" s="59">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s" s="60">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s" s="60">
+        <v>104</v>
+      </c>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s" s="34">
-        <v>83</v>
-      </c>
-      <c r="C10" t="s" s="35">
-        <v>84</v>
-      </c>
-      <c r="D10" t="s" s="35">
-        <v>85</v>
-      </c>
-      <c r="E10" s="8"/>
+      <c r="A10" t="s" s="56">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s" s="59">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s" s="60">
+        <v>106</v>
+      </c>
+      <c r="D10" t="s" s="60">
+        <v>107</v>
+      </c>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="36"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="8"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="8"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="8"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="8"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="27"/>
     </row>
     <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="27"/>
     </row>
     <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actual version of test switching regions
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/alx.xlsx
+++ b/src/test/resources/xls/alx.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="153">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -142,7 +142,7 @@
     <t>REG002</t>
   </si>
   <si>
-    <t>Brasil</t>
+    <t>Brazil (Brasil)</t>
   </si>
   <si>
     <t>REG003</t>
@@ -154,13 +154,13 @@
     <t>REG004</t>
   </si>
   <si>
-    <t>China</t>
+    <t>China (中国大陆)</t>
   </si>
   <si>
     <t>REG005</t>
   </si>
   <si>
-    <t>Egypt</t>
+    <t>Egypt (مصر)</t>
   </si>
   <si>
     <t>REG006</t>
@@ -172,7 +172,7 @@
     <t>REG007</t>
   </si>
   <si>
-    <t>Germany</t>
+    <t>Germany (Deutschland)</t>
   </si>
   <si>
     <t>REG008</t>
@@ -184,37 +184,37 @@
     <t>REG009</t>
   </si>
   <si>
-    <t>Italy</t>
+    <t>Italy (Italia)</t>
   </si>
   <si>
     <t>REG010</t>
   </si>
   <si>
-    <t>Japan</t>
+    <t>Japan (日本)</t>
   </si>
   <si>
     <t>REG011</t>
   </si>
   <si>
-    <t>Mexico</t>
+    <t>Mexico (México)</t>
   </si>
   <si>
     <t>REG012</t>
   </si>
   <si>
-    <t>Netherlands</t>
+    <t>Netherlands (Nederland)</t>
   </si>
   <si>
     <t>REG013</t>
   </si>
   <si>
-    <t>Poland</t>
+    <t>Poland (Polska)</t>
   </si>
   <si>
     <t>REG014</t>
   </si>
   <si>
-    <t>Saudi Arabia</t>
+    <t>Saudi Arabia (المملكة العربية السعودية)</t>
   </si>
   <si>
     <t>REG015</t>
@@ -226,31 +226,37 @@
     <t>REG016</t>
   </si>
   <si>
-    <t>Spain</t>
+    <t>Spain (España)</t>
   </si>
   <si>
     <t>REG017</t>
   </si>
   <si>
-    <t>Sweden</t>
+    <t>Sweden (Sverige)</t>
   </si>
   <si>
     <t>REG018</t>
   </si>
   <si>
+    <t>Turkey (Türkiye)</t>
+  </si>
+  <si>
+    <t>REG019</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>REG020</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>REG021</t>
+  </si>
+  <si>
     <t>United Arab Emirates</t>
-  </si>
-  <si>
-    <t>REG019</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>REG020</t>
-  </si>
-  <si>
-    <t>United States</t>
   </si>
   <si>
     <t>TUID</t>
@@ -633,7 +639,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -747,6 +753,17 @@
       <left style="thin">
         <color indexed="17"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
       <right style="thin">
         <color indexed="18"/>
       </right>
@@ -792,6 +809,15 @@
       <left style="thin">
         <color indexed="17"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
       <right style="thin">
         <color indexed="18"/>
       </right>
@@ -830,6 +856,17 @@
       </top>
       <bottom style="thin">
         <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -898,26 +935,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="17"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="13"/>
       </left>
       <right/>
@@ -968,7 +985,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1050,97 +1067,100 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1152,7 +1172,7 @@
     <xf numFmtId="49" fontId="6" fillId="9" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1161,19 +1181,19 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2555,15 +2575,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="15" style="25" customWidth="1"/>
-    <col min="2" max="3" width="16.3516" style="25" customWidth="1"/>
-    <col min="4" max="16384" width="16.3516" style="25" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="25" customWidth="1"/>
+    <col min="3" max="3" width="32.9141" style="25" customWidth="1"/>
+    <col min="4" max="5" width="16.3516" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="8.8" customHeight="1">
@@ -2576,226 +2598,281 @@
       <c r="C1" t="s" s="26">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" ht="13.1" customHeight="1">
-      <c r="A2" t="s" s="27">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s" s="28">
+      <c r="D1" s="27"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1">
+      <c r="A2" t="s" s="28">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="29">
         <v>22</v>
       </c>
-      <c r="C2" t="s" s="29">
+      <c r="C2" t="s" s="30">
         <v>23</v>
       </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" ht="13.1" customHeight="1">
-      <c r="A3" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s" s="31">
+      <c r="A3" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s" s="33">
         <v>24</v>
       </c>
-      <c r="C3" t="s" s="32">
+      <c r="C3" t="s" s="34">
         <v>25</v>
       </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" ht="12.9" customHeight="1">
-      <c r="A4" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s" s="31">
+      <c r="A4" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="33">
         <v>26</v>
       </c>
-      <c r="C4" t="s" s="32">
+      <c r="C4" t="s" s="34">
         <v>27</v>
       </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" ht="12.9" customHeight="1">
-      <c r="A5" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s" s="31">
+      <c r="A5" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="C5" t="s" s="32">
+      <c r="C5" t="s" s="34">
         <v>29</v>
       </c>
+      <c r="D5" s="31"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" ht="12.9" customHeight="1">
-      <c r="A6" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s" s="31">
+      <c r="A6" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s" s="33">
         <v>30</v>
       </c>
-      <c r="C6" t="s" s="32">
+      <c r="C6" t="s" s="34">
         <v>31</v>
       </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" ht="12.9" customHeight="1">
-      <c r="A7" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s" s="31">
+      <c r="A7" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s" s="33">
         <v>32</v>
       </c>
-      <c r="C7" t="s" s="32">
+      <c r="C7" t="s" s="34">
         <v>33</v>
       </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" ht="12.9" customHeight="1">
-      <c r="A8" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s" s="31">
+      <c r="A8" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s" s="33">
         <v>34</v>
       </c>
-      <c r="C8" t="s" s="32">
+      <c r="C8" t="s" s="34">
         <v>35</v>
       </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" ht="12.9" customHeight="1">
-      <c r="A9" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s" s="31">
+      <c r="A9" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" s="33">
         <v>36</v>
       </c>
-      <c r="C9" t="s" s="32">
+      <c r="C9" t="s" s="34">
         <v>37</v>
       </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" ht="12.9" customHeight="1">
-      <c r="A10" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s" s="31">
+      <c r="A10" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s" s="33">
         <v>38</v>
       </c>
-      <c r="C10" t="s" s="32">
+      <c r="C10" t="s" s="34">
         <v>39</v>
       </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" ht="12.9" customHeight="1">
-      <c r="A11" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s" s="31">
+      <c r="A11" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s" s="33">
         <v>40</v>
       </c>
-      <c r="C11" t="s" s="32">
+      <c r="C11" t="s" s="34">
         <v>41</v>
       </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" ht="12.9" customHeight="1">
-      <c r="A12" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s" s="31">
+      <c r="A12" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s" s="33">
         <v>42</v>
       </c>
-      <c r="C12" t="s" s="32">
+      <c r="C12" t="s" s="34">
         <v>43</v>
       </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" ht="12.9" customHeight="1">
-      <c r="A13" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s" s="31">
+      <c r="A13" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s" s="33">
         <v>44</v>
       </c>
-      <c r="C13" t="s" s="32">
+      <c r="C13" t="s" s="34">
         <v>45</v>
       </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" ht="12.9" customHeight="1">
-      <c r="A14" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s" s="31">
+      <c r="A14" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s" s="33">
         <v>46</v>
       </c>
-      <c r="C14" t="s" s="32">
+      <c r="C14" t="s" s="34">
         <v>47</v>
       </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" ht="12.9" customHeight="1">
-      <c r="A15" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s" s="31">
+      <c r="A15" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s" s="33">
         <v>48</v>
       </c>
-      <c r="C15" t="s" s="32">
+      <c r="C15" t="s" s="34">
         <v>49</v>
       </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" ht="12.9" customHeight="1">
-      <c r="A16" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s" s="31">
+      <c r="A16" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s" s="33">
         <v>50</v>
       </c>
-      <c r="C16" t="s" s="32">
+      <c r="C16" t="s" s="34">
         <v>51</v>
       </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" ht="12.9" customHeight="1">
-      <c r="A17" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s" s="31">
+      <c r="A17" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s" s="33">
         <v>52</v>
       </c>
-      <c r="C17" t="s" s="32">
+      <c r="C17" t="s" s="34">
         <v>53</v>
       </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" ht="12.9" customHeight="1">
-      <c r="A18" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s" s="31">
+      <c r="A18" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s" s="33">
         <v>54</v>
       </c>
-      <c r="C18" t="s" s="32">
+      <c r="C18" t="s" s="34">
         <v>55</v>
       </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" ht="12.9" customHeight="1">
-      <c r="A19" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s" s="31">
+      <c r="A19" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s" s="33">
         <v>56</v>
       </c>
-      <c r="C19" t="s" s="32">
+      <c r="C19" t="s" s="34">
         <v>57</v>
       </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" ht="12.9" customHeight="1">
-      <c r="A20" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s" s="31">
+      <c r="A20" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s" s="33">
         <v>58</v>
       </c>
-      <c r="C20" t="s" s="32">
+      <c r="C20" t="s" s="34">
         <v>59</v>
       </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" ht="12.9" customHeight="1">
-      <c r="A21" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s" s="31">
+      <c r="A21" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s" s="33">
         <v>60</v>
       </c>
-      <c r="C21" t="s" s="32">
+      <c r="C21" t="s" s="34">
         <v>61</v>
       </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" ht="12.9" customHeight="1">
+      <c r="A22" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s" s="33">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s" s="34">
+        <v>63</v>
+      </c>
+      <c r="D22" s="35"/>
+      <c r="E22" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -2814,190 +2891,190 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="33" customWidth="1"/>
-    <col min="2" max="2" width="15.3516" style="33" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="33" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="33" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="33" customWidth="1"/>
-    <col min="6" max="6" width="10.1719" style="33" customWidth="1"/>
-    <col min="7" max="7" width="11.8516" style="33" customWidth="1"/>
-    <col min="8" max="9" width="8.85156" style="33" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="33" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="36" customWidth="1"/>
+    <col min="2" max="2" width="15.3516" style="36" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="36" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="36" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="36" customWidth="1"/>
+    <col min="6" max="6" width="10.1719" style="36" customWidth="1"/>
+    <col min="7" max="7" width="11.8516" style="36" customWidth="1"/>
+    <col min="8" max="9" width="8.85156" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="34">
+      <c r="A1" t="s" s="37">
         <v>18</v>
       </c>
-      <c r="B1" t="s" s="34">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s" s="34">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s" s="34">
+      <c r="B1" t="s" s="37">
         <v>64</v>
       </c>
-      <c r="E1" t="s" s="34">
+      <c r="C1" t="s" s="37">
         <v>65</v>
       </c>
-      <c r="F1" t="s" s="34">
+      <c r="D1" t="s" s="37">
         <v>66</v>
       </c>
-      <c r="G1" t="s" s="34">
+      <c r="E1" t="s" s="37">
         <v>67</v>
       </c>
-      <c r="H1" t="s" s="34">
+      <c r="F1" t="s" s="37">
         <v>68</v>
       </c>
-      <c r="I1" s="35"/>
+      <c r="G1" t="s" s="37">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s" s="37">
+        <v>70</v>
+      </c>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" ht="16" customHeight="1">
-      <c r="A2" t="s" s="36">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s" s="36">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s" s="36">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s" s="37">
+      <c r="A2" t="s" s="39">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="39">
         <v>71</v>
       </c>
-      <c r="E2" t="s" s="36">
+      <c r="C2" t="s" s="39">
         <v>72</v>
       </c>
-      <c r="F2" t="s" s="36">
+      <c r="D2" t="s" s="40">
         <v>73</v>
       </c>
-      <c r="G2" t="s" s="36">
+      <c r="E2" t="s" s="39">
         <v>74</v>
       </c>
-      <c r="H2" t="s" s="36">
+      <c r="F2" t="s" s="39">
         <v>75</v>
       </c>
-      <c r="I2" s="38"/>
+      <c r="G2" t="s" s="39">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s" s="39">
+        <v>77</v>
+      </c>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="36">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s" s="36">
-        <v>76</v>
-      </c>
-      <c r="C3" t="s" s="36">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s" s="36">
-        <v>77</v>
-      </c>
-      <c r="E3" t="s" s="36">
+      <c r="A3" t="s" s="39">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s" s="39">
         <v>78</v>
       </c>
-      <c r="F3" t="s" s="36">
-        <v>73</v>
-      </c>
-      <c r="G3" t="s" s="36">
+      <c r="C3" t="s" s="39">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s" s="39">
         <v>79</v>
       </c>
-      <c r="H3" t="s" s="36">
+      <c r="E3" t="s" s="39">
         <v>80</v>
       </c>
-      <c r="I3" s="38"/>
+      <c r="F3" t="s" s="39">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s" s="39">
+        <v>81</v>
+      </c>
+      <c r="H3" t="s" s="39">
+        <v>82</v>
+      </c>
+      <c r="I3" s="41"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="36">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s" s="36">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s" s="36">
-        <v>70</v>
-      </c>
-      <c r="D4" t="s" s="36">
-        <v>82</v>
-      </c>
-      <c r="E4" t="s" s="36">
+      <c r="A4" t="s" s="39">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="39">
         <v>83</v>
       </c>
-      <c r="F4" t="s" s="36">
+      <c r="C4" t="s" s="39">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s" s="39">
         <v>84</v>
       </c>
-      <c r="G4" t="s" s="36">
+      <c r="E4" t="s" s="39">
         <v>85</v>
       </c>
-      <c r="H4" t="s" s="36">
+      <c r="F4" t="s" s="39">
         <v>86</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="G4" t="s" s="39">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s" s="39">
+        <v>88</v>
+      </c>
+      <c r="I4" s="41"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3019,8 +3096,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="39" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="39" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="42" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -3031,96 +3108,96 @@
         <v>19</v>
       </c>
       <c r="C1" t="s" s="26">
-        <v>87</v>
-      </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
+        <v>89</v>
+      </c>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" ht="13.1" customHeight="1">
-      <c r="A2" t="s" s="27">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s" s="28">
-        <v>88</v>
-      </c>
-      <c r="C2" s="42">
+      <c r="A2" t="s" s="28">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="29">
+        <v>90</v>
+      </c>
+      <c r="C2" s="45">
         <v>1234567</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" ht="12.9" customHeight="1">
-      <c r="A3" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s" s="31">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s" s="32">
-        <v>90</v>
-      </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="44"/>
+      <c r="A3" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s" s="33">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s" s="34">
+        <v>92</v>
+      </c>
+      <c r="D3" s="48"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" ht="12.9" customHeight="1">
-      <c r="A4" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s" s="31">
-        <v>91</v>
-      </c>
-      <c r="C4" t="s" s="32">
-        <v>92</v>
-      </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="44"/>
+      <c r="A4" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="33">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s" s="34">
+        <v>94</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="47"/>
     </row>
     <row r="5" ht="12.9" customHeight="1">
-      <c r="A5" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s" s="31">
-        <v>93</v>
-      </c>
-      <c r="C5" t="s" s="32">
-        <v>94</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="44"/>
+      <c r="A5" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="33">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s" s="34">
+        <v>96</v>
+      </c>
+      <c r="D5" s="48"/>
+      <c r="E5" s="47"/>
     </row>
     <row r="6" ht="12.9" customHeight="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="44"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="47"/>
     </row>
     <row r="7" ht="12.9" customHeight="1">
-      <c r="A7" s="46"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="44"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="47"/>
     </row>
     <row r="8" ht="12.9" customHeight="1">
-      <c r="A8" s="46"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="44"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="47"/>
     </row>
     <row r="9" ht="12.9" customHeight="1">
-      <c r="A9" s="46"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="44"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="47"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="48"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="21"/>
     </row>
   </sheetData>
@@ -3143,8 +3220,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="50" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="50" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -3155,114 +3232,114 @@
         <v>19</v>
       </c>
       <c r="C1" t="s" s="26">
-        <v>95</v>
-      </c>
-      <c r="D1" s="51"/>
+        <v>97</v>
+      </c>
+      <c r="D1" s="27"/>
       <c r="E1" s="9"/>
     </row>
     <row r="2" ht="13.1" customHeight="1">
-      <c r="A2" t="s" s="27">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s" s="28">
-        <v>96</v>
-      </c>
-      <c r="C2" t="s" s="29">
-        <v>97</v>
-      </c>
-      <c r="D2" s="52"/>
+      <c r="A2" t="s" s="28">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="29">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s" s="30">
+        <v>99</v>
+      </c>
+      <c r="D2" s="31"/>
       <c r="E2" s="12"/>
     </row>
     <row r="3" ht="12.9" customHeight="1">
-      <c r="A3" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s" s="31">
-        <v>98</v>
-      </c>
-      <c r="C3" t="s" s="32">
-        <v>99</v>
-      </c>
-      <c r="D3" s="52"/>
+      <c r="A3" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s" s="33">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s" s="34">
+        <v>101</v>
+      </c>
+      <c r="D3" s="31"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" ht="12.9" customHeight="1">
-      <c r="A4" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s" s="31">
-        <v>100</v>
-      </c>
-      <c r="C4" t="s" s="32">
-        <v>101</v>
-      </c>
-      <c r="D4" s="52"/>
+      <c r="A4" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="33">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s" s="34">
+        <v>103</v>
+      </c>
+      <c r="D4" s="31"/>
       <c r="E4" s="12"/>
     </row>
     <row r="5" ht="12.9" customHeight="1">
-      <c r="A5" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s" s="31">
-        <v>102</v>
-      </c>
-      <c r="C5" t="s" s="32">
-        <v>103</v>
-      </c>
-      <c r="D5" s="52"/>
+      <c r="A5" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="33">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s" s="34">
+        <v>105</v>
+      </c>
+      <c r="D5" s="31"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" ht="12.9" customHeight="1">
-      <c r="A6" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s" s="31">
-        <v>104</v>
-      </c>
-      <c r="C6" t="s" s="32">
-        <v>105</v>
-      </c>
-      <c r="D6" s="52"/>
+      <c r="A6" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s" s="33">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s" s="34">
+        <v>107</v>
+      </c>
+      <c r="D6" s="31"/>
       <c r="E6" s="12"/>
     </row>
     <row r="7" ht="12.9" customHeight="1">
-      <c r="A7" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s" s="31">
-        <v>106</v>
-      </c>
-      <c r="C7" t="s" s="32">
-        <v>107</v>
-      </c>
-      <c r="D7" s="52"/>
+      <c r="A7" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s" s="33">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s" s="34">
+        <v>109</v>
+      </c>
+      <c r="D7" s="31"/>
       <c r="E7" s="12"/>
     </row>
     <row r="8" ht="12.9" customHeight="1">
-      <c r="A8" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s" s="31">
-        <v>108</v>
-      </c>
-      <c r="C8" t="s" s="32">
-        <v>109</v>
-      </c>
-      <c r="D8" s="52"/>
+      <c r="A8" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s" s="33">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s" s="34">
+        <v>111</v>
+      </c>
+      <c r="D8" s="31"/>
       <c r="E8" s="12"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="20"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="21"/>
     </row>
   </sheetData>
@@ -3282,123 +3359,123 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="56" customWidth="1"/>
-    <col min="2" max="2" width="11.3516" style="56" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="56" customWidth="1"/>
-    <col min="4" max="4" width="12.8516" style="56" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="56" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="56" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="57" customWidth="1"/>
+    <col min="2" max="2" width="11.3516" style="57" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="57" customWidth="1"/>
+    <col min="4" max="4" width="12.8516" style="57" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="57" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="57" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="34">
+      <c r="A1" t="s" s="37">
         <v>18</v>
       </c>
-      <c r="B1" t="s" s="34">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s" s="34">
-        <v>110</v>
-      </c>
-      <c r="D1" t="s" s="34">
-        <v>111</v>
-      </c>
-      <c r="E1" t="s" s="34">
+      <c r="B1" t="s" s="37">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s" s="37">
         <v>112</v>
       </c>
+      <c r="D1" t="s" s="37">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s" s="37">
+        <v>114</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="36">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s" s="36">
-        <v>113</v>
-      </c>
-      <c r="C2" t="s" s="36">
-        <v>114</v>
-      </c>
-      <c r="D2" t="s" s="36">
+      <c r="A2" t="s" s="39">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="39">
         <v>115</v>
       </c>
-      <c r="E2" s="57">
+      <c r="C2" t="s" s="39">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s" s="39">
+        <v>117</v>
+      </c>
+      <c r="E2" s="58">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="36">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s" s="36">
-        <v>116</v>
-      </c>
-      <c r="C3" t="s" s="36">
-        <v>117</v>
-      </c>
-      <c r="D3" t="s" s="36">
+      <c r="A3" t="s" s="39">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s" s="39">
         <v>118</v>
       </c>
-      <c r="E3" s="57">
+      <c r="C3" t="s" s="39">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s" s="39">
+        <v>120</v>
+      </c>
+      <c r="E3" s="58">
         <v>23</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="36">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s" s="36">
-        <v>119</v>
-      </c>
-      <c r="C4" t="s" s="36">
-        <v>120</v>
-      </c>
-      <c r="D4" t="s" s="36">
+      <c r="A4" t="s" s="39">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="39">
         <v>121</v>
       </c>
-      <c r="E4" s="57">
+      <c r="C4" t="s" s="39">
+        <v>122</v>
+      </c>
+      <c r="D4" t="s" s="39">
+        <v>123</v>
+      </c>
+      <c r="E4" s="58">
         <v>100</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3417,261 +3494,261 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.17188" style="58" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="58" customWidth="1"/>
-    <col min="4" max="4" width="20.3516" style="58" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="58" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="58" customWidth="1"/>
+    <col min="1" max="1" width="7.17188" style="59" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="59" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="59" customWidth="1"/>
+    <col min="4" max="4" width="20.3516" style="59" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="59" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="59" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="59">
+      <c r="A1" t="s" s="60">
         <v>18</v>
       </c>
-      <c r="B1" t="s" s="60">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s" s="60">
-        <v>122</v>
-      </c>
-      <c r="D1" t="s" s="60">
-        <v>123</v>
-      </c>
-      <c r="E1" s="61"/>
+      <c r="B1" t="s" s="61">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s" s="61">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s" s="61">
+        <v>125</v>
+      </c>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s" s="63">
-        <v>124</v>
-      </c>
-      <c r="C2" t="s" s="64">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s" s="64">
+      <c r="A2" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="64">
         <v>126</v>
       </c>
-      <c r="E2" s="35"/>
+      <c r="C2" t="s" s="65">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s" s="65">
+        <v>128</v>
+      </c>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s" s="65">
-        <v>127</v>
-      </c>
-      <c r="C3" t="s" s="66">
-        <v>128</v>
-      </c>
-      <c r="D3" t="s" s="66">
+      <c r="A3" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s" s="66">
         <v>129</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="C3" t="s" s="67">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s" s="67">
+        <v>131</v>
+      </c>
+      <c r="E3" s="38"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s" s="65">
-        <v>130</v>
-      </c>
-      <c r="C4" t="s" s="66">
-        <v>131</v>
-      </c>
-      <c r="D4" t="s" s="66">
+      <c r="A4" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="66">
         <v>132</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="C4" t="s" s="67">
+        <v>133</v>
+      </c>
+      <c r="D4" t="s" s="67">
+        <v>134</v>
+      </c>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s" s="65">
-        <v>133</v>
-      </c>
-      <c r="C5" t="s" s="66">
-        <v>134</v>
-      </c>
-      <c r="D5" t="s" s="66">
+      <c r="A5" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="66">
         <v>135</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="C5" t="s" s="67">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s" s="67">
+        <v>137</v>
+      </c>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s" s="65">
-        <v>136</v>
-      </c>
-      <c r="C6" t="s" s="66">
-        <v>137</v>
-      </c>
-      <c r="D6" t="s" s="66">
+      <c r="A6" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s" s="66">
         <v>138</v>
       </c>
-      <c r="E6" s="35"/>
+      <c r="C6" t="s" s="67">
+        <v>139</v>
+      </c>
+      <c r="D6" t="s" s="67">
+        <v>140</v>
+      </c>
+      <c r="E6" s="38"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s" s="65">
-        <v>139</v>
-      </c>
-      <c r="C7" t="s" s="66">
-        <v>140</v>
-      </c>
-      <c r="D7" t="s" s="66">
+      <c r="A7" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s" s="66">
         <v>141</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="C7" t="s" s="67">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s" s="67">
+        <v>143</v>
+      </c>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s" s="65">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s" s="66">
-        <v>143</v>
-      </c>
-      <c r="D8" t="s" s="66">
+      <c r="A8" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s" s="66">
         <v>144</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="C8" t="s" s="67">
+        <v>145</v>
+      </c>
+      <c r="D8" t="s" s="67">
+        <v>146</v>
+      </c>
+      <c r="E8" s="38"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s" s="65">
-        <v>145</v>
-      </c>
-      <c r="C9" t="s" s="66">
-        <v>146</v>
-      </c>
-      <c r="D9" t="s" s="66">
+      <c r="A9" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" s="66">
         <v>147</v>
       </c>
-      <c r="E9" s="35"/>
+      <c r="C9" t="s" s="67">
+        <v>148</v>
+      </c>
+      <c r="D9" t="s" s="67">
+        <v>149</v>
+      </c>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="62">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s" s="65">
-        <v>148</v>
-      </c>
-      <c r="C10" t="s" s="66">
-        <v>149</v>
-      </c>
-      <c r="D10" t="s" s="66">
+      <c r="A10" t="s" s="63">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s" s="66">
         <v>150</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="C10" t="s" s="67">
+        <v>151</v>
+      </c>
+      <c r="D10" t="s" s="67">
+        <v>152</v>
+      </c>
+      <c r="E10" s="38"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="35"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="35"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="35"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="35"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="38"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="35"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="38"/>
     </row>
     <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="35"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="38"/>
     </row>
     <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="35"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="35"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="38"/>
     </row>
     <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="35"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="38"/>
     </row>
     <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="35"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="38"/>
     </row>
     <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="35"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="38"/>
     </row>
     <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="35"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="35"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="35"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>